<commit_message>
2 logistic regression runs done + svm fixes
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/Logistic Regression/Individual_Features_PCA Training Statistics.xlsx
+++ b/Output/Classifier Fitting/Logistic Regression/Individual_Features_PCA Training Statistics.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>563.8951697985332</v>
+        <v>425.0779544154803</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09393556051949578</v>
+        <v>0.0708109202757755</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9663501582542062</v>
+        <v>0.9580209895052474</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9115456563974466</v>
+        <v>0.9158759367194005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>